<commit_message>
Added transform functions to New Sensor script.
</commit_message>
<xml_diff>
--- a/scripts/New_Sensors.xlsx
+++ b/scripts/New_Sensors.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="240" yWindow="30" windowWidth="25740" windowHeight="13935"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Main" sheetId="4" r:id="rId1"/>
+    <sheet name="2014-07-08" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="208">
   <si>
     <t>Site Outdoor Temp</t>
   </si>
@@ -481,6 +482,165 @@
   </si>
   <si>
     <t>DHW Recirc Return Temp</t>
+  </si>
+  <si>
+    <t>Chugach View</t>
+  </si>
+  <si>
+    <t>anc_merril_temp</t>
+  </si>
+  <si>
+    <t>anc_merril_wind</t>
+  </si>
+  <si>
+    <t>Utilities/Fuel</t>
+  </si>
+  <si>
+    <t>Electric Meter</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>53805</t>
+  </si>
+  <si>
+    <t>Gas Meter West</t>
+  </si>
+  <si>
+    <t>Gas Meter East</t>
+  </si>
+  <si>
+    <t>Btu/hour</t>
+  </si>
+  <si>
+    <t>Gas Meter Total</t>
+  </si>
+  <si>
+    <t>53802</t>
+  </si>
+  <si>
+    <t>53804</t>
+  </si>
+  <si>
+    <t>AplusBplusCplusD</t>
+  </si>
+  <si>
+    <t>id_A_sync="53802", id_B="53804"</t>
+  </si>
+  <si>
+    <t>chuvw_gas_total</t>
+  </si>
+  <si>
+    <t>rate*0.096*3600.0</t>
+  </si>
+  <si>
+    <t>max_rate=1.5</t>
+  </si>
+  <si>
+    <t>Is Calc'd Field [6]</t>
+  </si>
+  <si>
+    <t>Calc or Transform Function [7]</t>
+  </si>
+  <si>
+    <t>Function Parameters [8]</t>
+  </si>
+  <si>
+    <t>rate*1010.0*3600.0</t>
+  </si>
+  <si>
+    <t>DHW to Bldg Temp</t>
+  </si>
+  <si>
+    <t>55439</t>
+  </si>
+  <si>
+    <t>55436</t>
+  </si>
+  <si>
+    <t>55437</t>
+  </si>
+  <si>
+    <t>55442</t>
+  </si>
+  <si>
+    <t>chuvw_dhw_circ_run</t>
+  </si>
+  <si>
+    <t>onOffID="55442"</t>
+  </si>
+  <si>
+    <t>Space Conditions, Occupancy</t>
+  </si>
+  <si>
+    <t>Snowmelt</t>
+  </si>
+  <si>
+    <t>1=Occupied 0=Vacant</t>
+  </si>
+  <si>
+    <t>Occupied Fraction</t>
+  </si>
+  <si>
+    <t>1st Floor Hall Occup State</t>
+  </si>
+  <si>
+    <t>1st Floor Hall Occup Fraction</t>
+  </si>
+  <si>
+    <t>2nd Floor Hall Occup State</t>
+  </si>
+  <si>
+    <t>2nd Floor Hall Occup Fraction</t>
+  </si>
+  <si>
+    <t>Snowmelt Circ Pump On/Off</t>
+  </si>
+  <si>
+    <t>DHW Circ Pump On/Off</t>
+  </si>
+  <si>
+    <t>Snowmelt Circ Pump Runtime</t>
+  </si>
+  <si>
+    <t>Snowmelt to Slab Temp</t>
+  </si>
+  <si>
+    <t>Snowmelt from Slab Temp</t>
+  </si>
+  <si>
+    <t>55446</t>
+  </si>
+  <si>
+    <t>55445</t>
+  </si>
+  <si>
+    <t>onOffID="55446"</t>
+  </si>
+  <si>
+    <t>onOffID="55445"</t>
+  </si>
+  <si>
+    <t>chuvw_occup_run_1</t>
+  </si>
+  <si>
+    <t>chuvw_occup_run_2</t>
+  </si>
+  <si>
+    <t>55444</t>
+  </si>
+  <si>
+    <t>chuvw_snow_circ_run</t>
+  </si>
+  <si>
+    <t>onOffID="55444"</t>
+  </si>
+  <si>
+    <t>55438</t>
+  </si>
+  <si>
+    <t>55440</t>
   </si>
 </sst>
 </file>
@@ -533,7 +693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -542,6 +702,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -843,10 +1007,491 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="9" max="9" width="33.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>176</v>
+      </c>
+      <c r="I5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
+        <v>176</v>
+      </c>
+      <c r="I6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7">
+        <v>40</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>168</v>
+      </c>
+      <c r="I7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" t="s">
+        <v>184</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" t="s">
+        <v>186</v>
+      </c>
+      <c r="E15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" t="s">
+        <v>187</v>
+      </c>
+      <c r="E16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F16">
+        <v>40</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C17" t="s">
+        <v>192</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>185</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>185</v>
+      </c>
+      <c r="F18">
+        <v>20</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>185</v>
+      </c>
+      <c r="F19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C20" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" t="s">
+        <v>185</v>
+      </c>
+      <c r="F20">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2427,7 +3072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2439,7 +3084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added Building Groups to models. Allowed searching on sensor ID.
</commit_message>
<xml_diff>
--- a/scripts/New_Sensors.xlsx
+++ b/scripts/New_Sensors.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="4" r:id="rId1"/>
-    <sheet name="2014-07-08" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="2014-07-15" sheetId="5" r:id="rId2"/>
+    <sheet name="2014-07-08" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="208">
   <si>
     <t>Site Outdoor Temp</t>
   </si>
@@ -1488,6 +1489,487 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="9" max="9" width="33.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>176</v>
+      </c>
+      <c r="I5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
+        <v>176</v>
+      </c>
+      <c r="I6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7">
+        <v>40</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>168</v>
+      </c>
+      <c r="I7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12">
+        <v>50</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" t="s">
+        <v>184</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14" t="s">
+        <v>184</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" t="s">
+        <v>186</v>
+      </c>
+      <c r="E15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" t="s">
+        <v>187</v>
+      </c>
+      <c r="E16" t="s">
+        <v>184</v>
+      </c>
+      <c r="F16">
+        <v>40</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>64</v>
+      </c>
+      <c r="I16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C17" t="s">
+        <v>192</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>185</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>185</v>
+      </c>
+      <c r="F18">
+        <v>20</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>185</v>
+      </c>
+      <c r="F19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C20" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" t="s">
+        <v>185</v>
+      </c>
+      <c r="F20">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3072,7 +3554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3084,7 +3566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
New Chugach View sensors.
</commit_message>
<xml_diff>
--- a/scripts/New_Sensors.xlsx
+++ b/scripts/New_Sensors.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="237">
   <si>
     <t>Site Outdoor Temp</t>
   </si>
@@ -642,6 +642,93 @@
   </si>
   <si>
     <t>55440</t>
+  </si>
+  <si>
+    <t>chuvw_firing_rate</t>
+  </si>
+  <si>
+    <t>chuvw_boilers_fired</t>
+  </si>
+  <si>
+    <t>chuvw_firing_rate_tot</t>
+  </si>
+  <si>
+    <t>chuvw_header_temp</t>
+  </si>
+  <si>
+    <t>chuvw_outdoor_temp</t>
+  </si>
+  <si>
+    <t>chuvw_header_setpoint</t>
+  </si>
+  <si>
+    <t>chuvw_boilers_online</t>
+  </si>
+  <si>
+    <t>chuvw_boiler1_status</t>
+  </si>
+  <si>
+    <t>chuvw_boiler2_status</t>
+  </si>
+  <si>
+    <t>chuvw_io_status</t>
+  </si>
+  <si>
+    <t>chuvw_lead_boiler</t>
+  </si>
+  <si>
+    <t>chuvw_fault_code</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>West Boilers Fired</t>
+  </si>
+  <si>
+    <t>West Boiler Firing Rate</t>
+  </si>
+  <si>
+    <t>West Boiler Total Firing Rate</t>
+  </si>
+  <si>
+    <t>West Header Temperature</t>
+  </si>
+  <si>
+    <t>West Header Setpoint</t>
+  </si>
+  <si>
+    <t>West Boilers Online</t>
+  </si>
+  <si>
+    <t>West Boiler 1 Status</t>
+  </si>
+  <si>
+    <t>West Boiler 2 Status</t>
+  </si>
+  <si>
+    <t>West Lead Boiler</t>
+  </si>
+  <si>
+    <t>West Boiler I/O Status</t>
+  </si>
+  <si>
+    <t>West Boiler Fault Code</t>
+  </si>
+  <si>
+    <t>chuvw_gas_use</t>
+  </si>
+  <si>
+    <t>West Boiler Gas Use</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>id_val="chuvw_firing_rate_tot", slope=30000.0</t>
   </si>
 </sst>
 </file>
@@ -1008,11 +1095,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1059,13 +1144,19 @@
         <v>155</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>156</v>
+        <v>212</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1073,13 +1164,19 @@
         <v>155</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>157</v>
+        <v>209</v>
+      </c>
+      <c r="C3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D3" t="s">
+        <v>220</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1087,22 +1184,19 @@
         <v>155</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>161</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>223</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>158</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
-        <v>171</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1110,25 +1204,19 @@
         <v>155</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>166</v>
+        <v>210</v>
       </c>
       <c r="C5" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="D5" t="s">
-        <v>164</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>158</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>176</v>
-      </c>
-      <c r="I5" t="s">
-        <v>172</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1136,25 +1224,28 @@
         <v>155</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>167</v>
+        <v>233</v>
       </c>
       <c r="C6" t="s">
-        <v>163</v>
+        <v>234</v>
       </c>
       <c r="D6" t="s">
         <v>164</v>
       </c>
       <c r="E6" t="s">
-        <v>158</v>
+        <v>4</v>
       </c>
       <c r="F6">
-        <v>30</v>
+        <v>40</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>176</v>
+        <v>235</v>
       </c>
       <c r="I6" t="s">
-        <v>172</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1162,28 +1253,19 @@
         <v>155</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>170</v>
+        <v>211</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
+        <v>225</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>158</v>
+        <v>4</v>
       </c>
       <c r="F7">
-        <v>40</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>168</v>
-      </c>
-      <c r="I7" t="s">
-        <v>169</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1191,19 +1273,19 @@
         <v>155</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>178</v>
+        <v>213</v>
       </c>
       <c r="C8" t="s">
-        <v>177</v>
+        <v>226</v>
       </c>
       <c r="D8" t="s">
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="F8">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1211,19 +1293,19 @@
         <v>155</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>179</v>
+        <v>214</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>227</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>220</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="F9">
-        <v>20</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1231,19 +1313,19 @@
         <v>155</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>180</v>
+        <v>215</v>
       </c>
       <c r="C10" t="s">
-        <v>154</v>
+        <v>228</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>30</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1251,19 +1333,19 @@
         <v>155</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>181</v>
+        <v>216</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>229</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>40</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1271,28 +1353,19 @@
         <v>155</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>182</v>
+        <v>218</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>230</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>221</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="F12">
-        <v>50</v>
-      </c>
-      <c r="G12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" t="s">
-        <v>183</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1300,19 +1373,19 @@
         <v>155</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="C13" t="s">
-        <v>188</v>
+        <v>231</v>
       </c>
       <c r="D13" t="s">
-        <v>186</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>184</v>
+        <v>4</v>
       </c>
       <c r="F13">
-        <v>10</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1320,166 +1393,19 @@
         <v>155</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="C14" t="s">
-        <v>189</v>
+        <v>232</v>
       </c>
       <c r="D14" t="s">
-        <v>187</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>184</v>
+        <v>4</v>
       </c>
       <c r="F14">
-        <v>20</v>
-      </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>64</v>
-      </c>
-      <c r="I14" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>155</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D15" t="s">
-        <v>186</v>
-      </c>
-      <c r="E15" t="s">
-        <v>184</v>
-      </c>
-      <c r="F15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>155</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C16" t="s">
-        <v>191</v>
-      </c>
-      <c r="D16" t="s">
-        <v>187</v>
-      </c>
-      <c r="E16" t="s">
-        <v>184</v>
-      </c>
-      <c r="F16">
-        <v>40</v>
-      </c>
-      <c r="G16" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>64</v>
-      </c>
-      <c r="I16" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>155</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C17" t="s">
-        <v>192</v>
-      </c>
-      <c r="D17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" t="s">
-        <v>185</v>
-      </c>
-      <c r="F17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>155</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="C18" t="s">
-        <v>194</v>
-      </c>
-      <c r="D18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" t="s">
-        <v>185</v>
-      </c>
-      <c r="F18">
-        <v>20</v>
-      </c>
-      <c r="G18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>64</v>
-      </c>
-      <c r="I18" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>155</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C19" t="s">
-        <v>195</v>
-      </c>
-      <c r="D19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" t="s">
-        <v>185</v>
-      </c>
-      <c r="F19">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>155</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C20" t="s">
-        <v>196</v>
-      </c>
-      <c r="D20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" t="s">
-        <v>185</v>
-      </c>
-      <c r="F20">
-        <v>40</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1972,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>